<commit_message>
modified:   assets/form/IP/AKSZT.xlsx 	modified:   assets/form/IP/AO.xlsx 	modified:   assets/form/IP/APUZT.xlsx 	modified:   assets/form/IP/RAZR.xlsx 	modified:   assets/form/IP/ZHIUR.xlsx 	modified:   lib/dbhelper_ip.dart 	modified:   lib/main.dart 	modified:   lib/model_ip.dart 	modified:   lib/object_detail_ip.dart 	modified:   pubspec.lock 	modified:   pubspec.yaml
</commit_message>
<xml_diff>
--- a/assets/form/IP/AKSZT.xlsx
+++ b/assets/form/IP/AKSZT.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\flutterDartProjects\nov1\assets\form\IP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67FFFB57-20C3-4F7A-86A4-DF4109FDE971}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C4446F4-AFDF-42B3-9BD7-4CDC3C72657A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="24735" yWindow="2820" windowWidth="15375" windowHeight="7875" xr2:uid="{A241382B-7DAD-4B31-8429-4124316E6400}"/>
+    <workbookView xWindow="22905" yWindow="3750" windowWidth="15375" windowHeight="7875" xr2:uid="{A241382B-7DAD-4B31-8429-4124316E6400}"/>
   </bookViews>
   <sheets>
     <sheet name="AKSZT" sheetId="1" r:id="rId1"/>
@@ -21,9 +21,9 @@
   </externalReferences>
   <definedNames>
     <definedName name="Data2">#REF!</definedName>
-    <definedName name="Z_0C2ABC7C_6EE5_44A5_88A6_D08D39B715BC_.wvu.PrintArea" localSheetId="0">AKSZT!$A$1:$K$50</definedName>
+    <definedName name="Z_0C2ABC7C_6EE5_44A5_88A6_D08D39B715BC_.wvu.PrintArea" localSheetId="0">AKSZT!$A$1:$K$48</definedName>
     <definedName name="Газопроводы">[1]Свод!$A$5:INDEX([1]Свод!$A$5:$A$2000,COUNTA([1]Свод!$A$5:$A$2000))</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">AKSZT!$A$1:$K$47</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">AKSZT!$A$1:$K$45</definedName>
   </definedNames>
   <calcPr calcId="181029" iterateDelta="1E-4"/>
   <extLst>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="46">
   <si>
     <t>(дата)</t>
   </si>
@@ -170,6 +170,15 @@
   </si>
   <si>
     <t>Приложение 8</t>
+  </si>
+  <si>
+    <t>Филиал</t>
+  </si>
+  <si>
+    <t>от</t>
+  </si>
+  <si>
+    <t>ИПИ</t>
   </si>
 </sst>
 </file>
@@ -179,7 +188,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-FC19]dd\ mmmm\ yyyy&quot; г.&quot;;@"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -188,45 +197,80 @@
     <font>
       <sz val="12"/>
       <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="204"/>
     </font>
     <font>
       <sz val="14"/>
       <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="204"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="204"/>
     </font>
     <font>
       <i/>
       <sz val="12"/>
       <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="204"/>
     </font>
     <font>
       <sz val="11.5"/>
       <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="204"/>
     </font>
     <font>
       <sz val="9"/>
       <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="204"/>
     </font>
     <font>
       <sz val="11"/>
       <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="204"/>
     </font>
     <font>
       <i/>
       <sz val="14"/>
       <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="204"/>
     </font>
     <font>
       <b/>
       <sz val="12"/>
       <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="204"/>
     </font>
     <font>
       <sz val="12"/>
       <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="14"/>
+      <color theme="0"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="204"/>
     </font>
   </fonts>
   <fills count="2">
@@ -237,7 +281,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -274,11 +318,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -316,9 +369,6 @@
     <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -326,60 +376,68 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -401,15 +459,17 @@
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
-      <sheetName val="Журнал1"/>
       <sheetName val="Справочник дефектов ИП"/>
       <sheetName val="Свод"/>
       <sheetName val="ЗП ГОСТ Р 51164-98"/>
+      <sheetName val="Акт о контроле сплошности"/>
+      <sheetName val="Журнал1"/>
+      <sheetName val="Акт на приемку уложенного тр."/>
+      <sheetName val="Разрешение"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2">
+      <sheetData sheetId="1">
         <row r="5">
           <cell r="A5" t="str">
             <v>АГНКС-1</v>
@@ -615,8 +675,21 @@
             <v>Итог Результат</v>
           </cell>
         </row>
+        <row r="46">
+          <cell r="A46"/>
+        </row>
+        <row r="47">
+          <cell r="A47"/>
+        </row>
+        <row r="48">
+          <cell r="A48"/>
+        </row>
       </sheetData>
-      <sheetData sheetId="3"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3" refreshError="1"/>
+      <sheetData sheetId="4" refreshError="1"/>
+      <sheetData sheetId="5" refreshError="1"/>
+      <sheetData sheetId="6" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -630,10 +703,19 @@
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0">
+        <row r="37">
+          <cell r="A37"/>
+          <cell r="C37"/>
+          <cell r="D37"/>
+          <cell r="E37"/>
+          <cell r="F37"/>
+        </row>
         <row r="88">
           <cell r="E88" t="str">
             <v>-</v>
           </cell>
+          <cell r="F88"/>
+          <cell r="G88"/>
         </row>
       </sheetData>
     </sheetDataSet>
@@ -941,10 +1023,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:L105"/>
+  <dimension ref="A1:L103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A22" zoomScale="115" zoomScaleNormal="100" zoomScaleSheetLayoutView="115" workbookViewId="0">
+      <selection activeCell="I26" sqref="I26:J26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -962,177 +1044,162 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="K1" s="20" t="s">
+      <c r="K1" s="19" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="K2" s="20" t="s">
+      <c r="K2" s="19" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="K3" s="20" t="s">
+      <c r="K3" s="19" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="19"/>
-      <c r="B4" s="19"/>
-      <c r="C4" s="19"/>
-      <c r="D4" s="19"/>
-      <c r="E4" s="21" t="s">
+    <row r="4" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A4" s="18"/>
+      <c r="B4" s="18"/>
+      <c r="C4" s="18"/>
+      <c r="D4" s="18"/>
+      <c r="E4" s="32" t="s">
         <v>39</v>
       </c>
-      <c r="F4" s="21"/>
-      <c r="G4" s="21"/>
-      <c r="H4" s="21"/>
-      <c r="I4" s="21"/>
-      <c r="J4" s="21"/>
-      <c r="K4" s="21"/>
-    </row>
-    <row r="5" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="19"/>
-      <c r="B5" s="19"/>
-      <c r="C5" s="19"/>
-      <c r="D5" s="19"/>
-      <c r="E5" s="22" t="s">
+      <c r="F4" s="32"/>
+      <c r="G4" s="32"/>
+      <c r="H4" s="32"/>
+      <c r="I4" s="32"/>
+      <c r="J4" s="32"/>
+      <c r="K4" s="32"/>
+    </row>
+    <row r="5" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A5" s="18"/>
+      <c r="B5" s="18"/>
+      <c r="C5" s="18"/>
+      <c r="D5" s="18"/>
+      <c r="E5" s="33"/>
+      <c r="F5" s="33"/>
+      <c r="G5" s="33"/>
+      <c r="H5" s="33"/>
+      <c r="I5" s="33"/>
+      <c r="J5" s="33"/>
+      <c r="K5" s="33"/>
+    </row>
+    <row r="6" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A6" s="18"/>
+      <c r="B6" s="18"/>
+      <c r="C6" s="18"/>
+      <c r="D6" s="18"/>
+      <c r="E6" s="33"/>
+      <c r="F6" s="33"/>
+      <c r="G6" s="33"/>
+      <c r="H6" s="33"/>
+      <c r="I6" s="33"/>
+      <c r="J6" s="33"/>
+      <c r="K6" s="33" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A7" s="18"/>
+      <c r="B7" s="18"/>
+      <c r="C7" s="18"/>
+      <c r="D7" s="18"/>
+      <c r="E7" s="33" t="s">
+        <v>38</v>
+      </c>
+      <c r="F7" s="33"/>
+      <c r="G7" s="33"/>
+      <c r="H7" s="33"/>
+      <c r="I7" s="33"/>
+      <c r="J7" s="33"/>
+      <c r="K7" s="33"/>
+    </row>
+    <row r="8" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A8" s="18"/>
+      <c r="B8" s="18"/>
+      <c r="C8" s="18"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="34"/>
+      <c r="F8" s="35"/>
+      <c r="G8" s="35"/>
+      <c r="H8" s="35"/>
+      <c r="I8" s="33"/>
+      <c r="J8" s="33"/>
+      <c r="K8" s="33"/>
+    </row>
+    <row r="9" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A9" s="18"/>
+      <c r="B9" s="18"/>
+      <c r="C9" s="18"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="36"/>
+      <c r="I9" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="F5" s="22"/>
-      <c r="G5" s="22"/>
-      <c r="H5" s="22"/>
-      <c r="I5" s="22"/>
-      <c r="J5" s="22"/>
-      <c r="K5" s="22"/>
-    </row>
-    <row r="6" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="19"/>
-      <c r="B6" s="19"/>
-      <c r="C6" s="19"/>
-      <c r="D6" s="19"/>
-      <c r="E6" s="22" t="s">
-        <v>3</v>
-      </c>
-      <c r="F6" s="22"/>
-      <c r="G6" s="22"/>
-      <c r="H6" s="22"/>
-      <c r="I6" s="22"/>
-      <c r="J6" s="22"/>
-      <c r="K6" s="22"/>
-    </row>
-    <row r="7" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="19"/>
-      <c r="B7" s="19"/>
-      <c r="C7" s="19"/>
-      <c r="D7" s="19"/>
-      <c r="E7" s="22" t="s">
-        <v>38</v>
-      </c>
-      <c r="F7" s="22"/>
-      <c r="G7" s="22"/>
-      <c r="H7" s="22"/>
-      <c r="I7" s="22"/>
-      <c r="J7" s="22"/>
-      <c r="K7" s="22"/>
-    </row>
-    <row r="8" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A8" s="19"/>
-      <c r="B8" s="19"/>
-      <c r="C8" s="19"/>
-      <c r="D8" s="19"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="23"/>
-      <c r="H8" s="23"/>
-      <c r="I8" s="23"/>
-      <c r="J8" s="24" t="s">
-        <v>3</v>
-      </c>
-      <c r="K8" s="24"/>
-    </row>
-    <row r="9" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="19"/>
-      <c r="B9" s="19"/>
-      <c r="C9" s="19"/>
-      <c r="D9" s="19"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="H9" s="27" t="s">
-        <v>3</v>
-      </c>
-      <c r="I9" s="27"/>
-      <c r="J9" s="27"/>
-      <c r="K9" s="16" t="s">
-        <v>3</v>
-      </c>
+      <c r="J9" s="37"/>
+      <c r="K9" s="37"/>
     </row>
     <row r="10" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="B10" s="28" t="s">
+      <c r="B10" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="C10" s="28"/>
-      <c r="D10" s="28"/>
-      <c r="E10" s="28"/>
-      <c r="F10" s="28"/>
-      <c r="G10" s="28"/>
-      <c r="H10" s="28"/>
-      <c r="I10" s="28"/>
-      <c r="J10" s="28"/>
-      <c r="K10" s="28"/>
-      <c r="L10" s="18"/>
+      <c r="C10" s="30"/>
+      <c r="D10" s="30"/>
+      <c r="E10" s="30"/>
+      <c r="F10" s="30"/>
+      <c r="G10" s="30"/>
+      <c r="H10" s="30"/>
+      <c r="I10" s="30"/>
+      <c r="J10" s="30"/>
+      <c r="K10" s="30"/>
+      <c r="L10" s="17"/>
     </row>
     <row r="11" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="29" t="s">
+      <c r="B11" s="38"/>
+      <c r="C11" s="38"/>
+      <c r="D11" s="38"/>
+      <c r="E11" s="38"/>
+      <c r="F11" s="38" t="s">
         <v>36</v>
       </c>
-      <c r="B11" s="29"/>
-      <c r="C11" s="29"/>
-      <c r="D11" s="29"/>
-      <c r="E11" s="29"/>
-      <c r="F11" s="29"/>
-      <c r="G11" s="29"/>
-      <c r="H11" s="29"/>
-      <c r="I11" s="29"/>
-      <c r="J11" s="29"/>
-      <c r="K11" s="29"/>
+      <c r="G11" s="38"/>
+      <c r="H11" s="38"/>
+      <c r="I11" s="38"/>
+      <c r="J11" s="38"/>
+      <c r="K11" s="38"/>
     </row>
     <row r="12" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="29" t="s">
+      <c r="B12" s="38" t="s">
         <v>35</v>
       </c>
-      <c r="B12" s="29"/>
-      <c r="C12" s="29"/>
-      <c r="D12" s="29"/>
-      <c r="E12" s="29"/>
-      <c r="F12" s="29"/>
-      <c r="G12" s="29"/>
-      <c r="H12" s="29"/>
-      <c r="I12" s="29"/>
-      <c r="J12" s="29"/>
-      <c r="K12" s="29"/>
+      <c r="C12" s="38"/>
+      <c r="D12" s="38"/>
+      <c r="E12" s="38"/>
+      <c r="F12" s="38"/>
+      <c r="G12" s="38"/>
+      <c r="H12" s="38"/>
+      <c r="I12" s="38"/>
+      <c r="J12" s="38"/>
+      <c r="K12" s="38"/>
     </row>
     <row r="13" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
-      <c r="D13" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="E13" s="27" t="s">
-        <v>3</v>
-      </c>
-      <c r="F13" s="27"/>
-      <c r="G13" s="27"/>
-      <c r="H13" s="16" t="s">
-        <v>3</v>
-      </c>
+      <c r="D13" s="40" t="s">
+        <v>44</v>
+      </c>
+      <c r="E13" s="39"/>
+      <c r="F13" s="39"/>
+      <c r="G13" s="39"/>
+      <c r="H13" s="16"/>
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
       <c r="K13" s="1"/>
@@ -1153,422 +1220,417 @@
       <c r="K14" s="5"/>
     </row>
     <row r="15" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="25" t="s">
+      <c r="B15" s="41"/>
+      <c r="C15" s="41"/>
+      <c r="D15" s="41"/>
+      <c r="E15" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="B15" s="25"/>
-      <c r="C15" s="25"/>
-      <c r="D15" s="25"/>
-      <c r="E15" s="25"/>
-      <c r="F15" s="25"/>
-      <c r="G15" s="25"/>
-      <c r="H15" s="25"/>
-      <c r="I15" s="25"/>
-      <c r="J15" s="25"/>
-      <c r="K15" s="25"/>
+      <c r="F15" s="41"/>
+      <c r="G15" s="41"/>
+      <c r="H15" s="41"/>
+      <c r="I15" s="41"/>
+      <c r="J15" s="41"/>
+      <c r="K15" s="41"/>
     </row>
     <row r="16" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="26" t="s">
+      <c r="A16" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="B16" s="26"/>
-      <c r="C16" s="26"/>
-      <c r="D16" s="26"/>
-      <c r="E16" s="26"/>
-      <c r="F16" s="26"/>
-      <c r="G16" s="26"/>
-      <c r="H16" s="26"/>
-      <c r="I16" s="26"/>
-      <c r="J16" s="26"/>
-      <c r="K16" s="26"/>
+      <c r="B16" s="29"/>
+      <c r="C16" s="29"/>
+      <c r="D16" s="29"/>
+      <c r="E16" s="29"/>
+      <c r="F16" s="29"/>
+      <c r="G16" s="29"/>
+      <c r="H16" s="29"/>
+      <c r="I16" s="29"/>
+      <c r="J16" s="29"/>
+      <c r="K16" s="29"/>
     </row>
     <row r="17" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="25" t="s">
+      <c r="B17" s="41"/>
+      <c r="C17" s="41"/>
+      <c r="D17" s="41"/>
+      <c r="E17" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="B17" s="25"/>
-      <c r="C17" s="25"/>
-      <c r="D17" s="25"/>
-      <c r="E17" s="25"/>
-      <c r="F17" s="25"/>
-      <c r="G17" s="25"/>
-      <c r="H17" s="25"/>
-      <c r="I17" s="25"/>
-      <c r="J17" s="25"/>
-      <c r="K17" s="25"/>
+      <c r="F17" s="41"/>
+      <c r="G17" s="41"/>
+      <c r="H17" s="41"/>
+      <c r="I17" s="41"/>
+      <c r="J17" s="41"/>
+      <c r="K17" s="41"/>
     </row>
     <row r="18" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="26" t="s">
+      <c r="A18" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="B18" s="26"/>
-      <c r="C18" s="26"/>
-      <c r="D18" s="26"/>
-      <c r="E18" s="26"/>
-      <c r="F18" s="26"/>
-      <c r="G18" s="26"/>
-      <c r="H18" s="26"/>
-      <c r="I18" s="26"/>
-      <c r="J18" s="26"/>
-      <c r="K18" s="26"/>
+      <c r="B18" s="29"/>
+      <c r="C18" s="29"/>
+      <c r="D18" s="29"/>
+      <c r="E18" s="29"/>
+      <c r="F18" s="29"/>
+      <c r="G18" s="29"/>
+      <c r="H18" s="29"/>
+      <c r="I18" s="29"/>
+      <c r="J18" s="29"/>
+      <c r="K18" s="29"/>
     </row>
     <row r="19" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="25" t="s">
+      <c r="B19" s="41"/>
+      <c r="C19" s="41"/>
+      <c r="D19" s="41"/>
+      <c r="E19" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="B19" s="25"/>
-      <c r="C19" s="25"/>
-      <c r="D19" s="25"/>
-      <c r="E19" s="25"/>
-      <c r="F19" s="25"/>
-      <c r="G19" s="25"/>
-      <c r="H19" s="25"/>
-      <c r="I19" s="25"/>
-      <c r="J19" s="25"/>
-      <c r="K19" s="25"/>
+      <c r="F19" s="41"/>
+      <c r="G19" s="41"/>
+      <c r="H19" s="41"/>
+      <c r="I19" s="41"/>
+      <c r="J19" s="41"/>
+      <c r="K19" s="41"/>
     </row>
     <row r="20" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="26" t="s">
+      <c r="A20" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="B20" s="26"/>
-      <c r="C20" s="26"/>
-      <c r="D20" s="26"/>
-      <c r="E20" s="26"/>
-      <c r="F20" s="26"/>
-      <c r="G20" s="26"/>
-      <c r="H20" s="26"/>
-      <c r="I20" s="26"/>
-      <c r="J20" s="26"/>
-      <c r="K20" s="26"/>
+      <c r="B20" s="29"/>
+      <c r="C20" s="29"/>
+      <c r="D20" s="29"/>
+      <c r="E20" s="29"/>
+      <c r="F20" s="29"/>
+      <c r="G20" s="29"/>
+      <c r="H20" s="29"/>
+      <c r="I20" s="29"/>
+      <c r="J20" s="29"/>
+      <c r="K20" s="29"/>
     </row>
     <row r="21" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="25" t="s">
+      <c r="A21" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="14"/>
+      <c r="G21" s="14"/>
+      <c r="H21" s="14"/>
+      <c r="I21" s="14"/>
+      <c r="J21" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="B21" s="25"/>
-      <c r="C21" s="25"/>
-      <c r="D21" s="25"/>
-      <c r="E21" s="25"/>
-      <c r="F21" s="25"/>
-      <c r="G21" s="25"/>
-      <c r="H21" s="25"/>
-      <c r="I21" s="25"/>
-      <c r="J21" s="25"/>
-      <c r="K21" s="25"/>
+      <c r="K21" s="1" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="22" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="26" t="s">
-        <v>33</v>
-      </c>
-      <c r="B22" s="26"/>
-      <c r="C22" s="26"/>
-      <c r="D22" s="26"/>
-      <c r="E22" s="26"/>
-      <c r="F22" s="26"/>
-      <c r="G22" s="26"/>
-      <c r="H22" s="26"/>
-      <c r="I22" s="26"/>
-      <c r="J22" s="26"/>
-      <c r="K22" s="26"/>
+      <c r="A22" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B22" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D22" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="F22" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="G22" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="H22" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J22" s="5"/>
+      <c r="K22" s="5"/>
     </row>
     <row r="23" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="15" t="s">
-        <v>32</v>
-      </c>
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
-      <c r="F23" s="14"/>
-      <c r="G23" s="14"/>
-      <c r="H23" s="14"/>
-      <c r="I23" s="14"/>
-      <c r="J23" s="13" t="s">
+      <c r="A23" s="30" t="s">
+        <v>45</v>
+      </c>
+      <c r="B23" s="30"/>
+      <c r="C23" s="30"/>
+      <c r="D23" s="30"/>
+      <c r="E23" s="30"/>
+      <c r="F23" s="30"/>
+      <c r="G23" s="30"/>
+      <c r="H23" s="30"/>
+      <c r="I23" s="30"/>
+      <c r="J23" s="30"/>
+      <c r="K23" s="30"/>
+    </row>
+    <row r="24" spans="1:11" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="29" t="s">
+        <v>26</v>
+      </c>
+      <c r="B24" s="29"/>
+      <c r="C24" s="29"/>
+      <c r="D24" s="29"/>
+      <c r="E24" s="29"/>
+      <c r="F24" s="29"/>
+      <c r="G24" s="29"/>
+      <c r="H24" s="29"/>
+      <c r="I24" s="29"/>
+      <c r="J24" s="29"/>
+      <c r="K24" s="29"/>
+    </row>
+    <row r="25" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B25" s="12"/>
+      <c r="C25" s="4"/>
+      <c r="D25" s="12"/>
+      <c r="E25" s="4"/>
+      <c r="F25" s="4"/>
+      <c r="G25" s="4"/>
+      <c r="H25" s="5"/>
+      <c r="I25" s="5"/>
+      <c r="J25" s="5"/>
+      <c r="K25" s="5"/>
+    </row>
+    <row r="26" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="22" t="str">
+        <f>CONCATENATE([2]APUZT!A37,[2]APUZT!C37,[2]APUZT!D37,[2]APUZT!E37,[2]APUZT!F37)</f>
+        <v/>
+      </c>
+      <c r="B26" s="22"/>
+      <c r="C26" s="22"/>
+      <c r="D26" s="22"/>
+      <c r="E26" s="22"/>
+      <c r="F26" s="22"/>
+      <c r="G26" s="22"/>
+      <c r="H26" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="I26" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="K23" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="B24" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="D24" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="E24" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="F24" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="G24" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="H24" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="I24" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="J24" s="5"/>
-      <c r="K24" s="5"/>
-    </row>
-    <row r="25" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="28" t="s">
-        <v>3</v>
-      </c>
-      <c r="B25" s="28"/>
-      <c r="C25" s="28"/>
-      <c r="D25" s="28"/>
-      <c r="E25" s="28"/>
-      <c r="F25" s="28"/>
-      <c r="G25" s="28"/>
-      <c r="H25" s="28"/>
-      <c r="I25" s="28"/>
-      <c r="J25" s="28"/>
-      <c r="K25" s="28"/>
-    </row>
-    <row r="26" spans="1:11" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="26" t="s">
-        <v>26</v>
-      </c>
-      <c r="B26" s="26"/>
-      <c r="C26" s="26"/>
-      <c r="D26" s="26"/>
-      <c r="E26" s="26"/>
-      <c r="F26" s="26"/>
-      <c r="G26" s="26"/>
-      <c r="H26" s="26"/>
-      <c r="I26" s="26"/>
-      <c r="J26" s="26"/>
-      <c r="K26" s="26"/>
-    </row>
-    <row r="27" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B27" s="12"/>
-      <c r="C27" s="4"/>
-      <c r="D27" s="12"/>
-      <c r="E27" s="4"/>
-      <c r="F27" s="4"/>
-      <c r="G27" s="4"/>
+      <c r="J26" s="30"/>
+      <c r="K26" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="B27" s="31"/>
+      <c r="C27" s="31"/>
+      <c r="D27" s="31"/>
+      <c r="E27" s="31"/>
+      <c r="F27" s="5"/>
+      <c r="G27" s="5"/>
       <c r="H27" s="5"/>
       <c r="I27" s="5"/>
       <c r="J27" s="5"/>
       <c r="K27" s="5"/>
     </row>
     <row r="28" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="25" t="str">
-        <f>CONCATENATE([2]APUZT!A37,[2]APUZT!C37,[2]APUZT!D37,[2]APUZT!E37,[2]APUZT!F37)</f>
-        <v/>
-      </c>
-      <c r="B28" s="25"/>
-      <c r="C28" s="25"/>
-      <c r="D28" s="25"/>
-      <c r="E28" s="25"/>
-      <c r="F28" s="25"/>
-      <c r="G28" s="25"/>
-      <c r="H28" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="I28" s="28" t="s">
+      <c r="A28" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B28" s="5"/>
+      <c r="C28" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="J28" s="28"/>
+      <c r="D28" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E28" s="5"/>
+      <c r="F28" s="30" t="s">
+        <v>3</v>
+      </c>
+      <c r="G28" s="30"/>
+      <c r="H28" s="30"/>
+      <c r="I28" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="J28" s="11" t="s">
+        <v>3</v>
+      </c>
       <c r="K28" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="30" t="s">
-        <v>22</v>
-      </c>
-      <c r="B29" s="30"/>
-      <c r="C29" s="30"/>
-      <c r="D29" s="30"/>
-      <c r="E29" s="30"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B29" s="5"/>
+      <c r="C29" s="5"/>
+      <c r="D29" s="5"/>
+      <c r="E29" s="5"/>
       <c r="F29" s="5"/>
-      <c r="G29" s="5"/>
-      <c r="H29" s="5"/>
-      <c r="I29" s="5"/>
-      <c r="J29" s="5"/>
-      <c r="K29" s="5"/>
+      <c r="G29" s="4"/>
+      <c r="H29" s="4"/>
+      <c r="I29" s="4"/>
+      <c r="J29" s="4"/>
+      <c r="K29" s="4"/>
     </row>
     <row r="30" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B30" s="5"/>
-      <c r="C30" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B30" s="4"/>
+      <c r="C30" s="10" t="s">
         <v>3</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E30" s="5"/>
-      <c r="F30" s="28" t="s">
+        <v>15</v>
+      </c>
+      <c r="E30" s="4"/>
+      <c r="F30" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="G30" s="28"/>
-      <c r="H30" s="28"/>
-      <c r="I30" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="J30" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="K30" s="5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B31" s="5"/>
-      <c r="C31" s="5"/>
-      <c r="D31" s="5"/>
-      <c r="E31" s="5"/>
-      <c r="F31" s="5"/>
-      <c r="G31" s="4"/>
-      <c r="H31" s="4"/>
-      <c r="I31" s="4"/>
-      <c r="J31" s="4"/>
-      <c r="K31" s="4"/>
+      <c r="G30" s="26"/>
+      <c r="H30" s="26"/>
+      <c r="I30" s="26"/>
+      <c r="J30" s="26"/>
+      <c r="K30" s="26"/>
+    </row>
+    <row r="31" spans="1:11" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="1"/>
+      <c r="B31" s="1"/>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
+      <c r="F31" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="G31" s="25"/>
+      <c r="H31" s="25"/>
+      <c r="I31" s="25"/>
+      <c r="J31" s="25"/>
+      <c r="K31" s="25"/>
     </row>
     <row r="32" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B32" s="4"/>
-      <c r="C32" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B32" s="5"/>
+      <c r="C32" s="5"/>
+      <c r="D32" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="D32" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E32" s="4"/>
-      <c r="F32" s="31" t="s">
-        <v>3</v>
-      </c>
-      <c r="G32" s="31"/>
-      <c r="H32" s="31"/>
-      <c r="I32" s="31"/>
-      <c r="J32" s="31"/>
-      <c r="K32" s="31"/>
-    </row>
-    <row r="33" spans="1:11" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="1"/>
-      <c r="B33" s="1"/>
-      <c r="C33" s="1"/>
-      <c r="D33" s="1"/>
-      <c r="E33" s="1"/>
-      <c r="F33" s="32" t="s">
-        <v>14</v>
-      </c>
-      <c r="G33" s="32"/>
-      <c r="H33" s="32"/>
-      <c r="I33" s="32"/>
-      <c r="J33" s="32"/>
-      <c r="K33" s="32"/>
+      <c r="E32" s="26"/>
+      <c r="F32" s="26"/>
+      <c r="G32" s="26"/>
+      <c r="H32" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="I32" s="5"/>
+      <c r="J32" s="5"/>
+      <c r="K32" s="5"/>
+    </row>
+    <row r="33" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B33" s="5"/>
+      <c r="C33" s="5"/>
+      <c r="D33" s="5"/>
+      <c r="E33" s="5"/>
+      <c r="F33" s="5"/>
+      <c r="G33" s="5"/>
+      <c r="H33" s="5"/>
+      <c r="I33" s="5"/>
+      <c r="J33" s="5"/>
+      <c r="K33" s="5"/>
     </row>
     <row r="34" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B34" s="5"/>
       <c r="C34" s="5"/>
-      <c r="D34" s="31" t="s">
-        <v>3</v>
-      </c>
-      <c r="E34" s="31"/>
-      <c r="F34" s="31"/>
-      <c r="G34" s="31"/>
-      <c r="H34" s="5" t="s">
-        <v>10</v>
-      </c>
+      <c r="D34" s="5"/>
+      <c r="E34" s="5"/>
+      <c r="F34" s="5"/>
+      <c r="G34" s="5"/>
+      <c r="H34" s="5"/>
       <c r="I34" s="5"/>
       <c r="J34" s="5"/>
       <c r="K34" s="5"/>
     </row>
     <row r="35" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B35" s="5"/>
-      <c r="C35" s="5"/>
-      <c r="D35" s="5"/>
-      <c r="E35" s="5"/>
-      <c r="F35" s="5"/>
-      <c r="G35" s="5"/>
-      <c r="H35" s="5"/>
-      <c r="I35" s="5"/>
-      <c r="J35" s="5"/>
-      <c r="K35" s="5"/>
-    </row>
-    <row r="36" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="B35" s="26"/>
+      <c r="C35" s="26"/>
+      <c r="D35" s="26"/>
+      <c r="E35" s="26"/>
+      <c r="F35" s="26"/>
+      <c r="G35" s="26"/>
+      <c r="H35" s="26"/>
+      <c r="I35" s="26"/>
+      <c r="J35" s="26"/>
+      <c r="K35" s="26"/>
+    </row>
+    <row r="36" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B36" s="5"/>
-      <c r="C36" s="5"/>
-      <c r="D36" s="5"/>
-      <c r="E36" s="5"/>
-      <c r="F36" s="5"/>
-      <c r="G36" s="5"/>
-      <c r="H36" s="5"/>
-      <c r="I36" s="5"/>
-      <c r="J36" s="5"/>
-      <c r="K36" s="5"/>
+        <v>11</v>
+      </c>
+      <c r="B36" s="1"/>
+      <c r="C36" s="1"/>
+      <c r="D36" s="27" t="s">
+        <v>3</v>
+      </c>
+      <c r="E36" s="27"/>
+      <c r="F36" s="27"/>
+      <c r="G36" s="27"/>
+      <c r="H36" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I36" s="1"/>
+      <c r="J36" s="1"/>
+      <c r="K36" s="1"/>
     </row>
     <row r="37" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="31" t="s">
-        <v>3</v>
-      </c>
-      <c r="B37" s="31"/>
-      <c r="C37" s="31"/>
-      <c r="D37" s="31"/>
-      <c r="E37" s="31"/>
-      <c r="F37" s="31"/>
-      <c r="G37" s="31"/>
-      <c r="H37" s="31"/>
-      <c r="I37" s="31"/>
-      <c r="J37" s="31"/>
-      <c r="K37" s="31"/>
-    </row>
-    <row r="38" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B37" s="1"/>
+      <c r="C37" s="1"/>
+      <c r="D37" s="1"/>
+      <c r="E37" s="8"/>
+      <c r="F37" s="8"/>
+      <c r="G37" s="8"/>
+      <c r="H37" s="8"/>
+      <c r="I37" s="8"/>
+      <c r="J37" s="8"/>
+      <c r="K37" s="8"/>
+    </row>
+    <row r="38" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
-      <c r="D38" s="33" t="s">
-        <v>3</v>
-      </c>
-      <c r="E38" s="33"/>
-      <c r="F38" s="33"/>
-      <c r="G38" s="33"/>
-      <c r="H38" s="1" t="s">
-        <v>10</v>
-      </c>
+      <c r="D38" s="1"/>
+      <c r="E38" s="1"/>
+      <c r="F38" s="1"/>
+      <c r="G38" s="1"/>
+      <c r="H38" s="1"/>
       <c r="I38" s="1"/>
       <c r="J38" s="1"/>
       <c r="K38" s="1"/>
     </row>
     <row r="39" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="9" t="s">
-        <v>9</v>
-      </c>
+      <c r="A39" s="1"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
       <c r="D39" s="1"/>
@@ -1580,195 +1642,193 @@
       <c r="J39" s="8"/>
       <c r="K39" s="8"/>
     </row>
-    <row r="40" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B40" s="1"/>
-      <c r="C40" s="1"/>
-      <c r="D40" s="1"/>
-      <c r="E40" s="1"/>
-      <c r="F40" s="1"/>
-      <c r="G40" s="1"/>
-      <c r="H40" s="1"/>
-      <c r="I40" s="1"/>
-      <c r="J40" s="1"/>
-      <c r="K40" s="1"/>
+    <row r="40" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="28" t="s">
+        <v>7</v>
+      </c>
+      <c r="B40" s="28"/>
+      <c r="C40" s="28"/>
+      <c r="D40" s="28"/>
+      <c r="E40" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="F40" s="22"/>
+      <c r="G40" s="22"/>
+      <c r="H40" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="I40" s="23"/>
+      <c r="J40" s="24" t="s">
+        <v>3</v>
+      </c>
+      <c r="K40" s="24"/>
     </row>
     <row r="41" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
       <c r="D41" s="1"/>
-      <c r="E41" s="8"/>
-      <c r="F41" s="8"/>
-      <c r="G41" s="8"/>
-      <c r="H41" s="8"/>
-      <c r="I41" s="8"/>
-      <c r="J41" s="8"/>
-      <c r="K41" s="8"/>
-    </row>
-    <row r="42" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="34" t="s">
-        <v>7</v>
-      </c>
-      <c r="B42" s="34"/>
-      <c r="C42" s="34"/>
-      <c r="D42" s="34"/>
-      <c r="E42" s="25" t="s">
+      <c r="E41" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="F41" s="20"/>
+      <c r="G41" s="20"/>
+      <c r="H41" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="I41" s="20"/>
+      <c r="J41" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="K41" s="20"/>
+    </row>
+    <row r="42" spans="1:11" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="B42" s="21"/>
+      <c r="C42" s="21"/>
+      <c r="D42" s="21"/>
+      <c r="E42" s="22" t="str">
+        <f>[2]APUZT!E88:G88</f>
+        <v>-</v>
+      </c>
+      <c r="F42" s="22"/>
+      <c r="G42" s="22"/>
+      <c r="H42" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="I42" s="23"/>
+      <c r="J42" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="F42" s="25"/>
-      <c r="G42" s="25"/>
-      <c r="H42" s="35" t="s">
-        <v>4</v>
-      </c>
-      <c r="I42" s="35"/>
-      <c r="J42" s="36" t="s">
-        <v>3</v>
-      </c>
-      <c r="K42" s="36"/>
+      <c r="K42" s="24"/>
     </row>
     <row r="43" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
       <c r="D43" s="1"/>
-      <c r="E43" s="37" t="s">
+      <c r="E43" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="F43" s="37"/>
-      <c r="G43" s="37"/>
-      <c r="H43" s="37" t="s">
+      <c r="F43" s="20"/>
+      <c r="G43" s="20"/>
+      <c r="H43" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="I43" s="37"/>
-      <c r="J43" s="37" t="s">
+      <c r="I43" s="20"/>
+      <c r="J43" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="K43" s="37"/>
-    </row>
-    <row r="44" spans="1:11" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="38" t="s">
-        <v>6</v>
-      </c>
-      <c r="B44" s="38"/>
-      <c r="C44" s="38"/>
-      <c r="D44" s="38"/>
-      <c r="E44" s="25" t="str">
-        <f>[2]APUZT!E88:G88</f>
-        <v>-</v>
-      </c>
-      <c r="F44" s="25"/>
-      <c r="G44" s="25"/>
-      <c r="H44" s="35" t="s">
+      <c r="K43" s="20"/>
+    </row>
+    <row r="44" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="B44" s="21"/>
+      <c r="C44" s="21"/>
+      <c r="D44" s="21"/>
+      <c r="E44" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="F44" s="22"/>
+      <c r="G44" s="22"/>
+      <c r="H44" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="I44" s="35"/>
-      <c r="J44" s="36" t="s">
+      <c r="I44" s="23"/>
+      <c r="J44" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="K44" s="36"/>
+      <c r="K44" s="24"/>
     </row>
     <row r="45" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="1"/>
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
       <c r="D45" s="1"/>
-      <c r="E45" s="37" t="s">
+      <c r="E45" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="F45" s="37"/>
-      <c r="G45" s="37"/>
-      <c r="H45" s="37" t="s">
+      <c r="F45" s="20"/>
+      <c r="G45" s="20"/>
+      <c r="H45" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="I45" s="37"/>
-      <c r="J45" s="37" t="s">
+      <c r="I45" s="20"/>
+      <c r="J45" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="K45" s="37"/>
-    </row>
-    <row r="46" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="38" t="s">
-        <v>5</v>
-      </c>
-      <c r="B46" s="38"/>
-      <c r="C46" s="38"/>
-      <c r="D46" s="38"/>
-      <c r="E46" s="25" t="s">
+      <c r="K45" s="20"/>
+    </row>
+    <row r="46" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="21" t="e">
+        <f>#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="B46" s="21"/>
+      <c r="C46" s="21"/>
+      <c r="D46" s="21"/>
+      <c r="E46" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="F46" s="25"/>
-      <c r="G46" s="25"/>
-      <c r="H46" s="35" t="s">
+      <c r="F46" s="22"/>
+      <c r="G46" s="22"/>
+      <c r="H46" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="I46" s="35"/>
-      <c r="J46" s="36" t="s">
+      <c r="I46" s="23"/>
+      <c r="J46" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="K46" s="36"/>
+      <c r="K46" s="24"/>
     </row>
     <row r="47" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="1"/>
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
       <c r="D47" s="1"/>
-      <c r="E47" s="37" t="s">
+      <c r="E47" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="F47" s="37"/>
-      <c r="G47" s="37"/>
-      <c r="H47" s="37" t="s">
+      <c r="F47" s="20"/>
+      <c r="G47" s="20"/>
+      <c r="H47" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="I47" s="37"/>
-      <c r="J47" s="37" t="s">
+      <c r="I47" s="20"/>
+      <c r="J47" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="K47" s="37"/>
-    </row>
-    <row r="48" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="38" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="B48" s="38"/>
-      <c r="C48" s="38"/>
-      <c r="D48" s="38"/>
-      <c r="E48" s="25" t="s">
-        <v>3</v>
-      </c>
-      <c r="F48" s="25"/>
-      <c r="G48" s="25"/>
-      <c r="H48" s="35" t="s">
-        <v>4</v>
-      </c>
-      <c r="I48" s="35"/>
-      <c r="J48" s="36" t="s">
-        <v>3</v>
-      </c>
-      <c r="K48" s="36"/>
+      <c r="K47" s="20"/>
+    </row>
+    <row r="48" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="1"/>
+      <c r="B48" s="1"/>
+      <c r="C48" s="1"/>
+      <c r="D48" s="1"/>
+      <c r="E48" s="1"/>
+      <c r="F48" s="1"/>
+      <c r="G48" s="1"/>
+      <c r="H48" s="1"/>
+      <c r="I48" s="1"/>
+      <c r="J48" s="1"/>
+      <c r="K48" s="1"/>
     </row>
     <row r="49" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="1"/>
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
       <c r="D49" s="1"/>
-      <c r="E49" s="37" t="s">
-        <v>2</v>
-      </c>
-      <c r="F49" s="37"/>
-      <c r="G49" s="37"/>
-      <c r="H49" s="37" t="s">
-        <v>1</v>
-      </c>
-      <c r="I49" s="37"/>
-      <c r="J49" s="37" t="s">
-        <v>0</v>
-      </c>
-      <c r="K49" s="37"/>
+      <c r="E49" s="1"/>
+      <c r="F49" s="1"/>
+      <c r="G49" s="1"/>
+      <c r="H49" s="1"/>
+      <c r="I49" s="1"/>
+      <c r="J49" s="1"/>
+      <c r="K49" s="1"/>
     </row>
     <row r="50" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="1"/>
@@ -1810,17 +1870,17 @@
       <c r="K52" s="1"/>
     </row>
     <row r="53" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="1"/>
-      <c r="B53" s="1"/>
-      <c r="C53" s="1"/>
-      <c r="D53" s="1"/>
-      <c r="E53" s="1"/>
-      <c r="F53" s="1"/>
-      <c r="G53" s="1"/>
-      <c r="H53" s="1"/>
-      <c r="I53" s="1"/>
-      <c r="J53" s="1"/>
-      <c r="K53" s="1"/>
+      <c r="A53" s="5"/>
+      <c r="B53" s="5"/>
+      <c r="C53" s="5"/>
+      <c r="D53" s="5"/>
+      <c r="E53" s="5"/>
+      <c r="F53" s="5"/>
+      <c r="G53" s="5"/>
+      <c r="H53" s="5"/>
+      <c r="I53" s="5"/>
+      <c r="J53" s="5"/>
+      <c r="K53" s="5"/>
     </row>
     <row r="54" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="1"/>
@@ -1836,17 +1896,17 @@
       <c r="K54" s="1"/>
     </row>
     <row r="55" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="5"/>
-      <c r="B55" s="5"/>
-      <c r="C55" s="5"/>
-      <c r="D55" s="5"/>
-      <c r="E55" s="5"/>
-      <c r="F55" s="5"/>
-      <c r="G55" s="5"/>
-      <c r="H55" s="5"/>
-      <c r="I55" s="5"/>
-      <c r="J55" s="5"/>
-      <c r="K55" s="5"/>
+      <c r="A55" s="1"/>
+      <c r="B55" s="1"/>
+      <c r="C55" s="1"/>
+      <c r="D55" s="1"/>
+      <c r="E55" s="1"/>
+      <c r="F55" s="1"/>
+      <c r="G55" s="1"/>
+      <c r="H55" s="1"/>
+      <c r="I55" s="1"/>
+      <c r="J55" s="1"/>
+      <c r="K55" s="1"/>
     </row>
     <row r="56" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="1"/>
@@ -1874,18 +1934,18 @@
       <c r="J57" s="1"/>
       <c r="K57" s="1"/>
     </row>
-    <row r="58" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="1"/>
-      <c r="B58" s="1"/>
-      <c r="C58" s="1"/>
-      <c r="D58" s="1"/>
-      <c r="E58" s="1"/>
-      <c r="F58" s="1"/>
-      <c r="G58" s="1"/>
-      <c r="H58" s="1"/>
-      <c r="I58" s="1"/>
-      <c r="J58" s="1"/>
-      <c r="K58" s="1"/>
+    <row r="58" spans="1:11" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="7"/>
+      <c r="B58" s="7"/>
+      <c r="C58" s="7"/>
+      <c r="D58" s="7"/>
+      <c r="E58" s="7"/>
+      <c r="F58" s="7"/>
+      <c r="G58" s="7"/>
+      <c r="H58" s="7"/>
+      <c r="I58" s="7"/>
+      <c r="J58" s="7"/>
+      <c r="K58" s="7"/>
     </row>
     <row r="59" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="1"/>
@@ -1900,18 +1960,18 @@
       <c r="J59" s="1"/>
       <c r="K59" s="1"/>
     </row>
-    <row r="60" spans="1:11" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="7"/>
-      <c r="B60" s="7"/>
-      <c r="C60" s="7"/>
-      <c r="D60" s="7"/>
-      <c r="E60" s="7"/>
-      <c r="F60" s="7"/>
-      <c r="G60" s="7"/>
-      <c r="H60" s="7"/>
-      <c r="I60" s="7"/>
-      <c r="J60" s="7"/>
-      <c r="K60" s="7"/>
+    <row r="60" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="1"/>
+      <c r="B60" s="1"/>
+      <c r="C60" s="1"/>
+      <c r="D60" s="1"/>
+      <c r="E60" s="1"/>
+      <c r="F60" s="1"/>
+      <c r="G60" s="1"/>
+      <c r="H60" s="1"/>
+      <c r="I60" s="1"/>
+      <c r="J60" s="1"/>
+      <c r="K60" s="1"/>
     </row>
     <row r="61" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="1"/>
@@ -1940,59 +2000,59 @@
       <c r="K62" s="1"/>
     </row>
     <row r="63" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="1"/>
-      <c r="B63" s="1"/>
-      <c r="C63" s="1"/>
-      <c r="D63" s="1"/>
-      <c r="E63" s="1"/>
-      <c r="F63" s="1"/>
-      <c r="G63" s="1"/>
-      <c r="H63" s="1"/>
-      <c r="I63" s="1"/>
-      <c r="J63" s="1"/>
-      <c r="K63" s="1"/>
+      <c r="A63" s="5"/>
+      <c r="B63" s="5"/>
+      <c r="C63" s="5"/>
+      <c r="D63" s="5"/>
+      <c r="E63" s="5"/>
+      <c r="F63" s="5"/>
+      <c r="G63" s="5"/>
+      <c r="H63" s="5"/>
+      <c r="I63" s="5"/>
+      <c r="J63" s="5"/>
+      <c r="K63" s="5"/>
     </row>
     <row r="64" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="1"/>
-      <c r="B64" s="1"/>
-      <c r="C64" s="1"/>
-      <c r="D64" s="1"/>
-      <c r="E64" s="1"/>
-      <c r="F64" s="1"/>
-      <c r="G64" s="1"/>
-      <c r="H64" s="1"/>
-      <c r="I64" s="1"/>
-      <c r="J64" s="1"/>
-      <c r="K64" s="1"/>
+      <c r="A64" s="5"/>
+      <c r="B64" s="5"/>
+      <c r="C64" s="5"/>
+      <c r="D64" s="5"/>
+      <c r="E64" s="5"/>
+      <c r="F64" s="5"/>
+      <c r="G64" s="5"/>
+      <c r="H64" s="5"/>
+      <c r="I64" s="5"/>
+      <c r="J64" s="5"/>
+      <c r="K64" s="5"/>
     </row>
     <row r="65" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="5"/>
-      <c r="B65" s="5"/>
-      <c r="C65" s="5"/>
-      <c r="D65" s="5"/>
-      <c r="E65" s="5"/>
-      <c r="F65" s="5"/>
-      <c r="G65" s="5"/>
-      <c r="H65" s="5"/>
-      <c r="I65" s="5"/>
-      <c r="J65" s="5"/>
-      <c r="K65" s="5"/>
+      <c r="A65" s="1"/>
+      <c r="B65" s="1"/>
+      <c r="C65" s="1"/>
+      <c r="D65" s="1"/>
+      <c r="E65" s="1"/>
+      <c r="F65" s="1"/>
+      <c r="G65" s="1"/>
+      <c r="H65" s="1"/>
+      <c r="I65" s="1"/>
+      <c r="J65" s="1"/>
+      <c r="K65" s="1"/>
     </row>
     <row r="66" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="5"/>
-      <c r="B66" s="5"/>
-      <c r="C66" s="5"/>
-      <c r="D66" s="5"/>
-      <c r="E66" s="5"/>
-      <c r="F66" s="5"/>
-      <c r="G66" s="5"/>
-      <c r="H66" s="5"/>
-      <c r="I66" s="5"/>
-      <c r="J66" s="5"/>
-      <c r="K66" s="5"/>
+      <c r="A66" s="1"/>
+      <c r="B66" s="1"/>
+      <c r="C66" s="1"/>
+      <c r="D66" s="1"/>
+      <c r="E66" s="1"/>
+      <c r="F66" s="1"/>
+      <c r="G66" s="1"/>
+      <c r="H66" s="1"/>
+      <c r="I66" s="1"/>
+      <c r="J66" s="1"/>
+      <c r="K66" s="1"/>
     </row>
     <row r="67" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="1"/>
+      <c r="A67" s="6"/>
       <c r="B67" s="1"/>
       <c r="C67" s="1"/>
       <c r="D67" s="1"/>
@@ -2018,7 +2078,7 @@
       <c r="K68" s="1"/>
     </row>
     <row r="69" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="6"/>
+      <c r="A69" s="1"/>
       <c r="B69" s="1"/>
       <c r="C69" s="1"/>
       <c r="D69" s="1"/>
@@ -2044,56 +2104,56 @@
       <c r="K70" s="1"/>
     </row>
     <row r="71" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="1"/>
-      <c r="B71" s="1"/>
-      <c r="C71" s="1"/>
-      <c r="D71" s="1"/>
-      <c r="E71" s="1"/>
-      <c r="F71" s="1"/>
-      <c r="G71" s="1"/>
-      <c r="H71" s="1"/>
-      <c r="I71" s="1"/>
-      <c r="J71" s="1"/>
-      <c r="K71" s="1"/>
+      <c r="A71" s="5"/>
+      <c r="B71" s="5"/>
+      <c r="C71" s="5"/>
+      <c r="D71" s="5"/>
+      <c r="E71" s="5"/>
+      <c r="F71" s="5"/>
+      <c r="G71" s="5"/>
+      <c r="H71" s="5"/>
+      <c r="I71" s="5"/>
+      <c r="J71" s="5"/>
+      <c r="K71" s="5"/>
     </row>
     <row r="72" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="1"/>
-      <c r="B72" s="1"/>
-      <c r="C72" s="1"/>
-      <c r="D72" s="1"/>
-      <c r="E72" s="1"/>
-      <c r="F72" s="1"/>
-      <c r="G72" s="1"/>
-      <c r="H72" s="1"/>
-      <c r="I72" s="1"/>
-      <c r="J72" s="1"/>
-      <c r="K72" s="1"/>
+      <c r="A72" s="5"/>
+      <c r="B72" s="5"/>
+      <c r="C72" s="5"/>
+      <c r="D72" s="5"/>
+      <c r="E72" s="5"/>
+      <c r="F72" s="5"/>
+      <c r="G72" s="5"/>
+      <c r="H72" s="5"/>
+      <c r="I72" s="5"/>
+      <c r="J72" s="5"/>
+      <c r="K72" s="5"/>
     </row>
     <row r="73" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="5"/>
-      <c r="B73" s="5"/>
-      <c r="C73" s="5"/>
-      <c r="D73" s="5"/>
-      <c r="E73" s="5"/>
-      <c r="F73" s="5"/>
-      <c r="G73" s="5"/>
-      <c r="H73" s="5"/>
-      <c r="I73" s="5"/>
-      <c r="J73" s="5"/>
-      <c r="K73" s="5"/>
+      <c r="A73" s="1"/>
+      <c r="B73" s="1"/>
+      <c r="C73" s="1"/>
+      <c r="D73" s="1"/>
+      <c r="E73" s="1"/>
+      <c r="F73" s="1"/>
+      <c r="G73" s="1"/>
+      <c r="H73" s="1"/>
+      <c r="I73" s="1"/>
+      <c r="J73" s="1"/>
+      <c r="K73" s="1"/>
     </row>
     <row r="74" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="5"/>
-      <c r="B74" s="5"/>
-      <c r="C74" s="5"/>
-      <c r="D74" s="5"/>
-      <c r="E74" s="5"/>
-      <c r="F74" s="5"/>
-      <c r="G74" s="5"/>
-      <c r="H74" s="5"/>
-      <c r="I74" s="5"/>
-      <c r="J74" s="5"/>
-      <c r="K74" s="5"/>
+      <c r="A74" s="1"/>
+      <c r="B74" s="1"/>
+      <c r="C74" s="1"/>
+      <c r="D74" s="1"/>
+      <c r="E74" s="1"/>
+      <c r="F74" s="1"/>
+      <c r="G74" s="1"/>
+      <c r="H74" s="1"/>
+      <c r="I74" s="1"/>
+      <c r="J74" s="1"/>
+      <c r="K74" s="1"/>
     </row>
     <row r="75" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="1"/>
@@ -2148,20 +2208,20 @@
       <c r="K78" s="1"/>
     </row>
     <row r="79" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="1"/>
-      <c r="B79" s="1"/>
-      <c r="C79" s="1"/>
-      <c r="D79" s="1"/>
-      <c r="E79" s="1"/>
-      <c r="F79" s="1"/>
-      <c r="G79" s="1"/>
-      <c r="H79" s="1"/>
-      <c r="I79" s="1"/>
-      <c r="J79" s="1"/>
-      <c r="K79" s="1"/>
+      <c r="A79" s="4"/>
+      <c r="B79" s="5"/>
+      <c r="C79" s="5"/>
+      <c r="D79" s="5"/>
+      <c r="E79" s="5"/>
+      <c r="F79" s="5"/>
+      <c r="G79" s="5"/>
+      <c r="H79" s="5"/>
+      <c r="I79" s="5"/>
+      <c r="J79" s="5"/>
+      <c r="K79" s="5"/>
     </row>
     <row r="80" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="1"/>
+      <c r="A80" s="4"/>
       <c r="B80" s="1"/>
       <c r="C80" s="1"/>
       <c r="D80" s="1"/>
@@ -2173,21 +2233,21 @@
       <c r="J80" s="1"/>
       <c r="K80" s="1"/>
     </row>
-    <row r="81" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="4"/>
-      <c r="B81" s="5"/>
-      <c r="C81" s="5"/>
-      <c r="D81" s="5"/>
-      <c r="E81" s="5"/>
-      <c r="F81" s="5"/>
-      <c r="G81" s="5"/>
-      <c r="H81" s="5"/>
-      <c r="I81" s="5"/>
-      <c r="J81" s="5"/>
-      <c r="K81" s="5"/>
+    <row r="81" spans="1:11" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A81" s="3"/>
+      <c r="B81" s="3"/>
+      <c r="C81" s="3"/>
+      <c r="D81" s="3"/>
+      <c r="E81" s="1"/>
+      <c r="F81" s="1"/>
+      <c r="G81" s="1"/>
+      <c r="H81" s="1"/>
+      <c r="I81" s="1"/>
+      <c r="J81" s="1"/>
+      <c r="K81" s="1"/>
     </row>
     <row r="82" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="4"/>
+      <c r="A82" s="1"/>
       <c r="B82" s="1"/>
       <c r="C82" s="1"/>
       <c r="D82" s="1"/>
@@ -2199,11 +2259,11 @@
       <c r="J82" s="1"/>
       <c r="K82" s="1"/>
     </row>
-    <row r="83" spans="1:11" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="3"/>
-      <c r="B83" s="3"/>
-      <c r="C83" s="3"/>
-      <c r="D83" s="3"/>
+    <row r="83" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A83" s="1"/>
+      <c r="B83" s="1"/>
+      <c r="C83" s="1"/>
+      <c r="D83" s="1"/>
       <c r="E83" s="1"/>
       <c r="F83" s="1"/>
       <c r="G83" s="1"/>
@@ -2225,7 +2285,7 @@
       <c r="J84" s="1"/>
       <c r="K84" s="1"/>
     </row>
-    <row r="85" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="1"/>
       <c r="B85" s="1"/>
       <c r="C85" s="1"/>
@@ -2251,7 +2311,7 @@
       <c r="J86" s="1"/>
       <c r="K86" s="1"/>
     </row>
-    <row r="87" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="1"/>
       <c r="B87" s="1"/>
       <c r="C87" s="1"/>
@@ -2277,7 +2337,7 @@
       <c r="J88" s="1"/>
       <c r="K88" s="1"/>
     </row>
-    <row r="89" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="1"/>
       <c r="B89" s="1"/>
       <c r="C89" s="1"/>
@@ -2316,31 +2376,31 @@
       <c r="J91" s="1"/>
       <c r="K91" s="1"/>
     </row>
-    <row r="92" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="1"/>
-      <c r="B92" s="1"/>
-      <c r="C92" s="1"/>
-      <c r="D92" s="1"/>
-      <c r="E92" s="1"/>
-      <c r="F92" s="1"/>
-      <c r="G92" s="1"/>
-      <c r="H92" s="1"/>
-      <c r="I92" s="1"/>
-      <c r="J92" s="1"/>
-      <c r="K92" s="1"/>
-    </row>
-    <row r="93" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A93" s="1"/>
-      <c r="B93" s="1"/>
-      <c r="C93" s="1"/>
-      <c r="D93" s="1"/>
-      <c r="E93" s="1"/>
-      <c r="F93" s="1"/>
-      <c r="G93" s="1"/>
-      <c r="H93" s="1"/>
-      <c r="I93" s="1"/>
-      <c r="J93" s="1"/>
-      <c r="K93" s="1"/>
+    <row r="92" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A92" s="2"/>
+      <c r="B92" s="2"/>
+      <c r="C92" s="2"/>
+      <c r="D92" s="2"/>
+      <c r="E92" s="2"/>
+      <c r="F92" s="2"/>
+      <c r="G92" s="2"/>
+      <c r="H92" s="2"/>
+      <c r="I92" s="2"/>
+      <c r="J92" s="2"/>
+      <c r="K92" s="2"/>
+    </row>
+    <row r="93" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A93" s="2"/>
+      <c r="B93" s="2"/>
+      <c r="C93" s="2"/>
+      <c r="D93" s="2"/>
+      <c r="E93" s="2"/>
+      <c r="F93" s="2"/>
+      <c r="G93" s="2"/>
+      <c r="H93" s="2"/>
+      <c r="I93" s="2"/>
+      <c r="J93" s="2"/>
+      <c r="K93" s="2"/>
     </row>
     <row r="94" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A94" s="2"/>
@@ -2381,33 +2441,33 @@
       <c r="J96" s="2"/>
       <c r="K96" s="2"/>
     </row>
-    <row r="97" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A97" s="2"/>
-      <c r="B97" s="2"/>
-      <c r="C97" s="2"/>
-      <c r="D97" s="2"/>
-      <c r="E97" s="2"/>
-      <c r="F97" s="2"/>
-      <c r="G97" s="2"/>
-      <c r="H97" s="2"/>
-      <c r="I97" s="2"/>
-      <c r="J97" s="2"/>
-      <c r="K97" s="2"/>
-    </row>
-    <row r="98" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A98" s="2"/>
-      <c r="B98" s="2"/>
-      <c r="C98" s="2"/>
-      <c r="D98" s="2"/>
-      <c r="E98" s="2"/>
-      <c r="F98" s="2"/>
-      <c r="G98" s="2"/>
-      <c r="H98" s="2"/>
-      <c r="I98" s="2"/>
-      <c r="J98" s="2"/>
-      <c r="K98" s="2"/>
-    </row>
-    <row r="99" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A97" s="1"/>
+      <c r="B97" s="1"/>
+      <c r="C97" s="1"/>
+      <c r="D97" s="1"/>
+      <c r="E97" s="1"/>
+      <c r="F97" s="1"/>
+      <c r="G97" s="1"/>
+      <c r="H97" s="1"/>
+      <c r="I97" s="1"/>
+      <c r="J97" s="1"/>
+      <c r="K97" s="1"/>
+    </row>
+    <row r="98" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A98" s="1"/>
+      <c r="B98" s="1"/>
+      <c r="C98" s="1"/>
+      <c r="D98" s="1"/>
+      <c r="E98" s="1"/>
+      <c r="F98" s="1"/>
+      <c r="G98" s="1"/>
+      <c r="H98" s="1"/>
+      <c r="I98" s="1"/>
+      <c r="J98" s="1"/>
+      <c r="K98" s="1"/>
+    </row>
+    <row r="99" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A99" s="1"/>
       <c r="B99" s="1"/>
       <c r="C99" s="1"/>
@@ -2420,7 +2480,7 @@
       <c r="J99" s="1"/>
       <c r="K99" s="1"/>
     </row>
-    <row r="100" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A100" s="1"/>
       <c r="B100" s="1"/>
       <c r="C100" s="1"/>
@@ -2472,47 +2532,42 @@
       <c r="J103" s="1"/>
       <c r="K103" s="1"/>
     </row>
-    <row r="104" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A104" s="1"/>
-      <c r="B104" s="1"/>
-      <c r="C104" s="1"/>
-      <c r="D104" s="1"/>
-      <c r="E104" s="1"/>
-      <c r="F104" s="1"/>
-      <c r="G104" s="1"/>
-      <c r="H104" s="1"/>
-      <c r="I104" s="1"/>
-      <c r="J104" s="1"/>
-      <c r="K104" s="1"/>
-    </row>
-    <row r="105" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A105" s="1"/>
-      <c r="B105" s="1"/>
-      <c r="C105" s="1"/>
-      <c r="D105" s="1"/>
-      <c r="E105" s="1"/>
-      <c r="F105" s="1"/>
-      <c r="G105" s="1"/>
-      <c r="H105" s="1"/>
-      <c r="I105" s="1"/>
-      <c r="J105" s="1"/>
-      <c r="K105" s="1"/>
-    </row>
   </sheetData>
-  <mergeCells count="58">
-    <mergeCell ref="E49:G49"/>
-    <mergeCell ref="H49:I49"/>
-    <mergeCell ref="J49:K49"/>
-    <mergeCell ref="E47:G47"/>
-    <mergeCell ref="H47:I47"/>
-    <mergeCell ref="J47:K47"/>
-    <mergeCell ref="A48:D48"/>
-    <mergeCell ref="E48:G48"/>
-    <mergeCell ref="H48:I48"/>
-    <mergeCell ref="J48:K48"/>
-    <mergeCell ref="E45:G45"/>
-    <mergeCell ref="H45:I45"/>
-    <mergeCell ref="J45:K45"/>
+  <mergeCells count="51">
+    <mergeCell ref="E4:K4"/>
+    <mergeCell ref="E5:K5"/>
+    <mergeCell ref="E6:K6"/>
+    <mergeCell ref="E7:K7"/>
+    <mergeCell ref="E8:H8"/>
+    <mergeCell ref="I8:K8"/>
+    <mergeCell ref="A16:K16"/>
+    <mergeCell ref="A18:K18"/>
+    <mergeCell ref="B10:K10"/>
+    <mergeCell ref="E13:G13"/>
+    <mergeCell ref="I9:K9"/>
+    <mergeCell ref="A26:G26"/>
+    <mergeCell ref="I26:J26"/>
+    <mergeCell ref="A27:E27"/>
+    <mergeCell ref="F28:H28"/>
+    <mergeCell ref="F30:K30"/>
+    <mergeCell ref="A20:K20"/>
+    <mergeCell ref="A23:K23"/>
+    <mergeCell ref="A24:K24"/>
+    <mergeCell ref="F31:K31"/>
+    <mergeCell ref="D32:G32"/>
+    <mergeCell ref="A35:K35"/>
+    <mergeCell ref="D36:G36"/>
+    <mergeCell ref="A40:D40"/>
+    <mergeCell ref="E40:G40"/>
+    <mergeCell ref="H40:I40"/>
+    <mergeCell ref="J40:K40"/>
+    <mergeCell ref="E41:G41"/>
+    <mergeCell ref="H41:I41"/>
+    <mergeCell ref="J41:K41"/>
+    <mergeCell ref="A42:D42"/>
+    <mergeCell ref="E42:G42"/>
+    <mergeCell ref="H42:I42"/>
+    <mergeCell ref="J42:K42"/>
     <mergeCell ref="A46:D46"/>
     <mergeCell ref="E46:G46"/>
     <mergeCell ref="H46:I46"/>
@@ -2524,42 +2579,14 @@
     <mergeCell ref="E44:G44"/>
     <mergeCell ref="H44:I44"/>
     <mergeCell ref="J44:K44"/>
-    <mergeCell ref="F33:K33"/>
-    <mergeCell ref="D34:G34"/>
-    <mergeCell ref="A37:K37"/>
-    <mergeCell ref="D38:G38"/>
-    <mergeCell ref="A42:D42"/>
-    <mergeCell ref="E42:G42"/>
-    <mergeCell ref="H42:I42"/>
-    <mergeCell ref="J42:K42"/>
-    <mergeCell ref="A20:K20"/>
-    <mergeCell ref="A21:K21"/>
-    <mergeCell ref="A22:K22"/>
-    <mergeCell ref="A25:K25"/>
-    <mergeCell ref="A26:K26"/>
-    <mergeCell ref="A28:G28"/>
-    <mergeCell ref="I28:J28"/>
-    <mergeCell ref="A29:E29"/>
-    <mergeCell ref="F30:H30"/>
-    <mergeCell ref="F32:K32"/>
-    <mergeCell ref="H9:J9"/>
-    <mergeCell ref="B10:K10"/>
-    <mergeCell ref="A11:K11"/>
-    <mergeCell ref="A12:K12"/>
-    <mergeCell ref="E13:G13"/>
-    <mergeCell ref="A15:K15"/>
-    <mergeCell ref="A16:K16"/>
-    <mergeCell ref="A17:K17"/>
-    <mergeCell ref="A18:K18"/>
-    <mergeCell ref="A19:K19"/>
-    <mergeCell ref="E4:K4"/>
-    <mergeCell ref="E5:K5"/>
-    <mergeCell ref="E6:K6"/>
-    <mergeCell ref="E7:K7"/>
-    <mergeCell ref="G8:I8"/>
-    <mergeCell ref="J8:K8"/>
+    <mergeCell ref="E47:G47"/>
+    <mergeCell ref="H47:I47"/>
+    <mergeCell ref="J47:K47"/>
+    <mergeCell ref="E45:G45"/>
+    <mergeCell ref="H45:I45"/>
+    <mergeCell ref="J45:K45"/>
   </mergeCells>
   <pageMargins left="0.78750000000000009" right="0.78750000000000009" top="0.74791666666666701" bottom="0.74791666666666701" header="0.51181102362204689" footer="0.51181102362204689"/>
-  <pageSetup paperSize="9" scale="93" fitToHeight="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" scale="90" fitToHeight="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>